<commit_message>
all stable file version 1.0.0.0
</commit_message>
<xml_diff>
--- a/ExcelSheets/LR.xlsx
+++ b/ExcelSheets/LR.xlsx
@@ -1017,7 +1017,7 @@
       <c r="B8" s="23" t="n"/>
       <c r="C8" s="14" t="inlineStr">
         <is>
-          <t>PEOPLE TEST</t>
+          <t>DEFFTEST</t>
         </is>
       </c>
       <c r="D8" s="2" t="inlineStr">
@@ -1207,13 +1207,21 @@
           <t>Net</t>
         </is>
       </c>
-      <c r="F17" s="12" t="inlineStr"/>
+      <c r="F17" s="12" t="inlineStr">
+        <is>
+          <t>HGFJ</t>
+        </is>
+      </c>
       <c r="G17" s="13" t="inlineStr">
         <is>
           <t>Invoice No:</t>
         </is>
       </c>
-      <c r="H17" s="50" t="inlineStr"/>
+      <c r="H17" s="50" t="inlineStr">
+        <is>
+          <t>HGJ</t>
+        </is>
+      </c>
       <c r="I17" s="24" t="n"/>
     </row>
     <row r="18" ht="15" customHeight="1" s="20" thickBot="1">
@@ -1228,7 +1236,11 @@
           <t>Eway bill No:</t>
         </is>
       </c>
-      <c r="H18" s="50" t="inlineStr"/>
+      <c r="H18" s="50" t="inlineStr">
+        <is>
+          <t>JFHJ</t>
+        </is>
+      </c>
       <c r="I18" s="24" t="n"/>
     </row>
     <row r="19" ht="15" customHeight="1" s="20" thickBot="1">
@@ -1237,7 +1249,11 @@
           <t>Container No</t>
         </is>
       </c>
-      <c r="B19" s="52" t="n"/>
+      <c r="B19" s="52" t="inlineStr">
+        <is>
+          <t>HJXCZH</t>
+        </is>
+      </c>
       <c r="C19" s="29" t="n"/>
       <c r="D19" s="60" t="n"/>
       <c r="E19" s="4" t="n"/>
@@ -1247,7 +1263,11 @@
           <t>Remarks</t>
         </is>
       </c>
-      <c r="H19" s="22" t="inlineStr"/>
+      <c r="H19" s="22" t="inlineStr">
+        <is>
+          <t>GFDVHJK</t>
+        </is>
+      </c>
       <c r="I19" s="29" t="n"/>
     </row>
     <row r="20" ht="32.45" customHeight="1" s="20" thickBot="1">
@@ -1256,7 +1276,7 @@
           <t>Seal No.</t>
         </is>
       </c>
-      <c r="B20" s="58" t="n"/>
+      <c r="B20" s="58" t="inlineStr"/>
       <c r="C20" s="32" t="n"/>
       <c r="D20" s="61" t="n"/>
       <c r="E20" s="6" t="n"/>

</xml_diff>